<commit_message>
site finalizado faltando apenas integrações de pagamento e onboard
</commit_message>
<xml_diff>
--- a/Backlog Kairos.xlsx
+++ b/Backlog Kairos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.santos_sankh\Desktop\kairos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B332AF-F2AD-4DF2-97A8-05249F3463B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3875BFB5-06FC-4D76-8E29-339D2309BEC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7BBEEEC4-CEBE-45CD-B774-85F745F54761}"/>
+    <workbookView xWindow="28680" yWindow="2610" windowWidth="20640" windowHeight="11040" xr2:uid="{7BBEEEC4-CEBE-45CD-B774-85F745F54761}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>BACKLOG KAIROS SYSTEM</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>Andamento</t>
+  </si>
+  <si>
+    <t>Sistema Completo</t>
+  </si>
+  <si>
+    <t>Criar Gameficação</t>
   </si>
 </sst>
 </file>
@@ -669,7 +675,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:F14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -863,22 +869,22 @@
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="8">
+      <c r="A11" s="12">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="8" t="s">
+      <c r="D11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
@@ -917,25 +923,35 @@
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="8">
+      <c r="A14" s="12">
         <v>12</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="15"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="A15" s="15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>